<commit_message>
Lab11 v1.0 RELEASE (with graphics and all shit)
</commit_message>
<xml_diff>
--- a/KMZI_Lab11/Runtime_Lab11.xlsx
+++ b/KMZI_Lab11/Runtime_Lab11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valda\source\repos\semester#6\КМЗИ\KMZI_Lab11\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF653233-471A-446A-949C-D98EB32D168E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0BE9729-4C58-4A75-BE8A-7B385FAA74F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-104" yWindow="-104" windowWidth="22326" windowHeight="12200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -247,6 +247,60 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="ru-BY"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx2">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$B$3:$B$7</c:f>
@@ -364,6 +418,60 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="ru-BY"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx2">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$B$3:$B$7</c:f>
@@ -420,8 +528,9 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -1442,7 +1551,7 @@
   <dimension ref="B2:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>